<commit_message>
Implemented sequences, allowing us to
do whatever transfers we want to do, including hiding. It will now automatically calculate everything for whatever the sequence is, and whatever the carrier frequency and detuning.
</commit_message>
<xml_diff>
--- a/S12D52.xlsx
+++ b/S12D52.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Desktop\Repositories\Barium_Shelving-Adiabatic-Passage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF2EE7A-AF8F-456E-97CD-F8DAE6FE1407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F043DCB6-0FE8-4D2E-B3E1-2783856F9C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10806" yWindow="-120" windowWidth="8100" windowHeight="11910" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1038" yWindow="-96" windowWidth="22098" windowHeight="13152" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encoding-Choice" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="179">
   <si>
     <t>D52</t>
   </si>
@@ -467,13 +467,118 @@
   </si>
   <si>
     <t>b1st:2-1.p1:n1</t>
+  </si>
+  <si>
+    <t>Freqs</t>
+  </si>
+  <si>
+    <t>Care</t>
+  </si>
+  <si>
+    <t>1.n1:n1</t>
+  </si>
+  <si>
+    <t>1.p0:p0</t>
+  </si>
+  <si>
+    <t>2-1.p2:n1</t>
+  </si>
+  <si>
+    <t>2-1.n2:p0</t>
+  </si>
+  <si>
+    <t>2-1.p0:p0</t>
+  </si>
+  <si>
+    <t>2-1.p2:p0</t>
+  </si>
+  <si>
+    <t>1.p1:p1</t>
+  </si>
+  <si>
+    <t>2-1.n1:p1</t>
+  </si>
+  <si>
+    <t>2-1.p1:p1</t>
+  </si>
+  <si>
+    <t>1-2.p0:n2</t>
+  </si>
+  <si>
+    <t>2.n2:n2</t>
+  </si>
+  <si>
+    <t>1-2.n1:n1</t>
+  </si>
+  <si>
+    <t>1-2.p1:n1</t>
+  </si>
+  <si>
+    <t>2.n1:n1</t>
+  </si>
+  <si>
+    <t>1-2.p0:p0</t>
+  </si>
+  <si>
+    <t>2.p0:p0</t>
+  </si>
+  <si>
+    <t>1-2.n1:p1</t>
+  </si>
+  <si>
+    <t>1-2.p1:p1</t>
+  </si>
+  <si>
+    <t>2.p1:p1</t>
+  </si>
+  <si>
+    <t>1-2.p0:p2</t>
+  </si>
+  <si>
+    <t>2.p2:p2</t>
+  </si>
+  <si>
+    <t>To sort while keeping colors, copy COL S, T to COL U, V, then sort COL U, V. Colors won't move unless you do this every time you change Carrier Freq.</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>^Always 0.776MHz  from freq. of -2:-2</t>
+  </si>
+  <si>
+    <t>&lt;Always 1.783MHz from freq +2:+2</t>
+  </si>
+  <si>
+    <t>Yellow are relevant for only d=7</t>
+  </si>
+  <si>
+    <t>Red are relevant for both d=5 and d=7</t>
+  </si>
+  <si>
+    <t>Blue are relevant for only d=5</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>and 2.4844MHz from freq +1:+1</t>
+  </si>
+  <si>
+    <t>and 2.7133MHz from n1:n1</t>
+  </si>
+  <si>
+    <t>Within 1.5+2MHz:</t>
+  </si>
+  <si>
+    <t>Within 1.5+4MHz:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,8 +627,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,6 +742,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -967,7 +1092,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1147,6 +1272,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2767,10 +2904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z102"/>
+  <dimension ref="A1:AC102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L77" sqref="L77"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2784,12 +2921,41 @@
     <col min="18" max="18" width="12.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q2" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="X2" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2798,17 +2964,87 @@
       </c>
       <c r="O3" s="25"/>
       <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q3">
+        <f>F27</f>
+        <v>4020.0506474032709</v>
+      </c>
+      <c r="R3" s="13">
+        <f>ABS(Q3)</f>
+        <v>4020.0506474032709</v>
+      </c>
+      <c r="S3" s="13">
+        <f>$R$3</f>
+        <v>4020.0506474032709</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="U3" s="95">
+        <f>$R$28</f>
+        <v>3950.7847914522836</v>
+      </c>
+      <c r="V3" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="X3" s="95">
+        <f>$R$28</f>
+        <v>3950.7847914522836</v>
+      </c>
+      <c r="Y3" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA3" s="95">
+        <v>3892.7847914522836</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="F4" t="s">
         <v>11</v>
       </c>
       <c r="O4" s="25"/>
       <c r="P4" s="25"/>
-      <c r="Q4" s="36"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q4">
+        <f>F28</f>
+        <v>4023.3449247417011</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4:R66" si="0">ABS(Q4)</f>
+        <v>4023.3449247417011</v>
+      </c>
+      <c r="S4" s="14">
+        <f>$R$5</f>
+        <v>4026.6365039681605</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="U4" s="7">
+        <f>$R$35</f>
+        <v>3954.2770923921671</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="W4">
+        <f>U4-U3</f>
+        <v>3.4923009398835347</v>
+      </c>
+      <c r="X4" s="7">
+        <f>$R$35</f>
+        <v>3954.2770923921671</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z4">
+        <f>X4-X3</f>
+        <v>3.4923009398835347</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>3896.2770923921671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2821,15 +3057,48 @@
       <c r="N5" s="25"/>
       <c r="O5" s="25"/>
       <c r="P5" s="25"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q5">
+        <f>F29</f>
+        <v>4026.6365039681605</v>
+      </c>
+      <c r="R5" s="14">
+        <f t="shared" si="0"/>
+        <v>4026.6365039681605</v>
+      </c>
+      <c r="S5" s="27">
+        <f>$R$7</f>
+        <v>4011.1135903949094</v>
+      </c>
+      <c r="T5" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="U5" s="95">
+        <f>$R$37</f>
+        <v>3960.8629489570567</v>
+      </c>
+      <c r="V5" s="95" t="s">
+        <v>158</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ref="W5:W32" si="1">U5-U4</f>
+        <v>6.5858565648895819</v>
+      </c>
+      <c r="X5" s="95">
+        <f>$R$37</f>
+        <v>3960.8629489570567</v>
+      </c>
+      <c r="Y5" s="95" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" ref="Z5:Z32" si="2">X5-X4</f>
+        <v>6.5858565648895819</v>
+      </c>
+      <c r="AA5" s="29">
+        <v>3902.8629489570567</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>-1092</v>
       </c>
@@ -2842,15 +3111,48 @@
       <c r="N6" s="25"/>
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q6">
+        <f>F30</f>
+        <v>-4007.8166082986891</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>4007.8166082986891</v>
+      </c>
+      <c r="S6" s="29">
+        <f>$R$9</f>
+        <v>4017.6994469597994</v>
+      </c>
+      <c r="T6" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="U6" s="7">
+        <f>$R$44</f>
+        <v>3964.7328551226683</v>
+      </c>
+      <c r="V6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="1"/>
+        <v>3.86990616561161</v>
+      </c>
+      <c r="X6" s="7">
+        <f>$R$44</f>
+        <v>3964.7328551226683</v>
+      </c>
+      <c r="Y6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="2"/>
+        <v>3.86990616561161</v>
+      </c>
+      <c r="AA6" s="27">
+        <v>3906.7328551226683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="G7" s="2" t="s">
         <v>9</v>
       </c>
@@ -2860,15 +3162,48 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
       <c r="P7" s="25"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q7">
+        <f>F31</f>
+        <v>-4011.1135903949094</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="0"/>
+        <v>4011.1135903949094</v>
+      </c>
+      <c r="S7" s="32">
+        <f>$R$12</f>
+        <v>4037.3215678899123</v>
+      </c>
+      <c r="T7" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="U7" s="95">
+        <f>$R$51</f>
+        <v>3968.8370189222896</v>
+      </c>
+      <c r="V7" s="95" t="s">
+        <v>162</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="1"/>
+        <v>4.1041637996213467</v>
+      </c>
+      <c r="X7" s="95">
+        <f>$R$51</f>
+        <v>3968.8370189222896</v>
+      </c>
+      <c r="Y7" s="95" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="2"/>
+        <v>4.1041637996213467</v>
+      </c>
+      <c r="AA7" s="29">
+        <v>3910.8370189222896</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="F8" s="2">
         <v>-1</v>
       </c>
@@ -2896,15 +3231,48 @@
       <c r="N8" s="25"/>
       <c r="O8" s="25"/>
       <c r="P8" s="25"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q8">
+        <f>F32</f>
+        <v>-4014.4078677333391</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>4014.4078677333391</v>
+      </c>
+      <c r="S8" s="29">
+        <f>$R$14</f>
+        <v>3993.8399651504778</v>
+      </c>
+      <c r="T8" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="U8" s="7">
+        <f>$R$53</f>
+        <v>3975.4228754871792</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="1"/>
+        <v>6.5858565648895819</v>
+      </c>
+      <c r="X8" s="7">
+        <f>$R$53</f>
+        <v>3975.4228754871792</v>
+      </c>
+      <c r="Y8" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="2"/>
+        <v>6.5858565648895819</v>
+      </c>
+      <c r="AA8" s="27">
+        <v>3917.4228754871792</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2938,15 +3306,52 @@
       <c r="N9" s="25"/>
       <c r="O9" s="25"/>
       <c r="P9" s="25"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q9">
+        <f>F33</f>
+        <v>-4017.6994469597994</v>
+      </c>
+      <c r="R9" s="95">
+        <f t="shared" si="0"/>
+        <v>4017.6994469597994</v>
+      </c>
+      <c r="S9" s="27">
+        <f>$R$16</f>
+        <v>4000.4312245851279</v>
+      </c>
+      <c r="T9" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="U9" s="95">
+        <f>$R$60</f>
+        <v>3979.6874940795597</v>
+      </c>
+      <c r="V9" s="95" t="s">
+        <v>165</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="1"/>
+        <v>4.2646185923804296</v>
+      </c>
+      <c r="X9" s="95">
+        <f>$R$60</f>
+        <v>3979.6874940795597</v>
+      </c>
+      <c r="Y9" s="95" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="2"/>
+        <v>4.2646185923804296</v>
+      </c>
+      <c r="AA9" s="29">
+        <v>3921.6874940795597</v>
+      </c>
+      <c r="AB9">
+        <f>ABS($AA$10-AA9)</f>
+        <v>40.363153323711231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D10" s="2">
         <v>-1</v>
       </c>
@@ -2954,49 +3359,86 @@
         <v>-5020.2998688990901</v>
       </c>
       <c r="F10" s="13">
-        <f t="shared" ref="F10:M17" si="0">F$9-$E10 +$A$6</f>
+        <f t="shared" ref="F10:M17" si="3">F$9-$E10 +$A$6</f>
         <v>4020.0506474032709</v>
       </c>
       <c r="G10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4034.0272905514821</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4047.5649295146177</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3947.4905141138534</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3954.2770923921671</v>
       </c>
       <c r="K10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3961.4385777842381</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3968.8370189222896</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3976.3932167411294</v>
       </c>
       <c r="N10" s="25"/>
       <c r="O10" s="25"/>
       <c r="P10" s="25"/>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q10">
+        <f>F34</f>
+        <v>-4020.9883346929491</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>4020.9883346929491</v>
+      </c>
+      <c r="S10" s="29">
+        <f>$R$18</f>
+        <v>4007.0116915447379</v>
+      </c>
+      <c r="T10" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="U10" s="13">
+        <f>$R$3</f>
+        <v>4020.0506474032709</v>
+      </c>
+      <c r="V10" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="1"/>
+        <v>40.363153323711231</v>
+      </c>
+      <c r="X10" s="13">
+        <f>$R$3</f>
+        <v>4020.0506474032709</v>
+      </c>
+      <c r="Y10" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="2"/>
+        <v>40.363153323711231</v>
+      </c>
+      <c r="AA10" s="32">
+        <v>3962.0506474032709</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" ref="AB10:AB11" si="4">ABS($AA$10-AA10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
@@ -3013,49 +3455,90 @@
         <v>-5023.5941462375204</v>
       </c>
       <c r="F11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4023.3449247417011</v>
       </c>
       <c r="G11" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4037.3215678899123</v>
       </c>
       <c r="H11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4050.8592068530488</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3950.7847914522836</v>
       </c>
       <c r="J11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3957.5713697305973</v>
       </c>
       <c r="K11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3964.7328551226683</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3972.1312962607199</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3979.6874940795597</v>
       </c>
       <c r="N11" s="25"/>
       <c r="O11" s="25"/>
       <c r="P11" s="25"/>
-      <c r="Q11" s="36"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q11">
+        <f>G27</f>
+        <v>4034.0272905514821</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>4034.0272905514821</v>
+      </c>
+      <c r="S11" s="28">
+        <f>$R$19</f>
+        <v>4047.5649295146177</v>
+      </c>
+      <c r="T11" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="U11" s="14">
+        <f>$R$5</f>
+        <v>4026.6365039681605</v>
+      </c>
+      <c r="V11" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="1"/>
+        <v>6.5858565648895819</v>
+      </c>
+      <c r="X11" s="14">
+        <f>$R$5</f>
+        <v>4026.6365039681605</v>
+      </c>
+      <c r="Y11" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="2"/>
+        <v>6.5858565648895819</v>
+      </c>
+      <c r="AA11" s="28">
+        <v>3968.6365039681605</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="4"/>
+        <v>6.5858565648895819</v>
+      </c>
+      <c r="AC11">
+        <f>ABS($AA$12-AA11)</f>
+        <v>10.685063921751862</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" s="2">
         <v>1</v>
       </c>
@@ -3063,49 +3546,86 @@
         <v>-5026.8857254639797</v>
       </c>
       <c r="F12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4026.6365039681605</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4040.6131471163717</v>
       </c>
       <c r="H12" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4054.1507860795082</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3954.0763706787429</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3960.8629489570567</v>
       </c>
       <c r="K12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3968.0244343491277</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3975.4228754871792</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3982.979073306019</v>
       </c>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
       <c r="P12" s="25"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q12">
+        <f>G28</f>
+        <v>4037.3215678899123</v>
+      </c>
+      <c r="R12" s="13">
+        <f t="shared" si="0"/>
+        <v>4037.3215678899123</v>
+      </c>
+      <c r="S12" s="32">
+        <f>$R$21</f>
+        <v>4054.1507860795082</v>
+      </c>
+      <c r="T12" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="U12" s="32">
+        <f>$R$12</f>
+        <v>4037.3215678899123</v>
+      </c>
+      <c r="V12" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="1"/>
+        <v>10.685063921751862</v>
+      </c>
+      <c r="X12" s="32">
+        <f>$R$12</f>
+        <v>4037.3215678899123</v>
+      </c>
+      <c r="Y12" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="2"/>
+        <v>10.685063921751862</v>
+      </c>
+      <c r="AA12" s="32">
+        <v>3979.3215678899123</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" ref="AC12:AC13" si="5">ABS($AA$12-AA12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="2">
         <v>-2</v>
       </c>
@@ -3113,39 +3633,87 @@
         <v>3007.5673868028698</v>
       </c>
       <c r="F13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4007.8166082986891</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3993.8399651504778</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3980.3023261873418</v>
       </c>
       <c r="I13" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4080.3767415881071</v>
       </c>
       <c r="J13" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4073.5901633097928</v>
       </c>
       <c r="K13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4066.4286779177219</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4059.0302367796708</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4051.4740389608301</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q13">
+        <f>G29</f>
+        <v>4040.6131471163717</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>4040.6131471163717</v>
+      </c>
+      <c r="S13" s="95">
+        <f>$R$23</f>
+        <v>3983.5993082835621</v>
+      </c>
+      <c r="T13" s="95" t="s">
+        <v>153</v>
+      </c>
+      <c r="U13" s="28">
+        <f>$R$19</f>
+        <v>4047.5649295146177</v>
+      </c>
+      <c r="V13" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="1"/>
+        <v>10.243361624705358</v>
+      </c>
+      <c r="X13" s="28">
+        <f>$R$19</f>
+        <v>4047.5649295146177</v>
+      </c>
+      <c r="Y13" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="2"/>
+        <v>10.243361624705358</v>
+      </c>
+      <c r="AA13" s="14">
+        <v>3989.5649295146177</v>
+      </c>
+      <c r="AB13">
+        <f>ABS($AA$14-AA13)</f>
+        <v>6.5858565648904914</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="5"/>
+        <v>10.243361624705358</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="2">
         <v>-1</v>
       </c>
@@ -3153,39 +3721,83 @@
         <v>3010.8643688990901</v>
       </c>
       <c r="F14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4011.1135903949094</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3997.1369472466981</v>
       </c>
       <c r="H14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3983.5993082835621</v>
       </c>
       <c r="I14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4083.6737236843273</v>
       </c>
       <c r="J14" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4076.8871454060131</v>
       </c>
       <c r="K14" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4069.7256600139422</v>
       </c>
       <c r="L14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4062.327218875891</v>
       </c>
       <c r="M14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4054.7710210570503</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q14">
+        <f>G30</f>
+        <v>-3993.8399651504778</v>
+      </c>
+      <c r="R14" s="95">
+        <f t="shared" si="0"/>
+        <v>3993.8399651504778</v>
+      </c>
+      <c r="S14" s="7">
+        <f>$R$25</f>
+        <v>3990.1851648484521</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="U14" s="32">
+        <f>$R$21</f>
+        <v>4054.1507860795082</v>
+      </c>
+      <c r="V14" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="1"/>
+        <v>6.5858565648904914</v>
+      </c>
+      <c r="X14" s="32">
+        <f>$R$21</f>
+        <v>4054.1507860795082</v>
+      </c>
+      <c r="Y14" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="2"/>
+        <v>6.5858565648904914</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>3996.1507860795082</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" ref="AB14:AB15" si="6">ABS($AA$14-AA14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="9" t="s">
         <v>2</v>
       </c>
@@ -3202,39 +3814,83 @@
         <v>3014.1586462375199</v>
       </c>
       <c r="F15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4014.4078677333391</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4000.4312245851279</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3986.8935856219919</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4086.9680010227571</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4080.1814227444429</v>
       </c>
       <c r="K15" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4073.0199373523719</v>
       </c>
       <c r="L15" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4065.6214962143208</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4058.0652983954801</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q15">
+        <f>G31</f>
+        <v>-3997.1369472466981</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>3997.1369472466981</v>
+      </c>
+      <c r="S15" s="95">
+        <f>$R$28</f>
+        <v>3950.7847914522836</v>
+      </c>
+      <c r="T15" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="U15" s="95">
+        <f>$R$23</f>
+        <v>3983.5993082835621</v>
+      </c>
+      <c r="V15" s="95" t="s">
+        <v>153</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="1"/>
+        <v>-70.551477795946084</v>
+      </c>
+      <c r="X15" s="95">
+        <f>$R$23</f>
+        <v>3983.5993082835621</v>
+      </c>
+      <c r="Y15" s="95" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="2"/>
+        <v>-70.551477795946084</v>
+      </c>
+      <c r="AA15" s="16">
+        <v>4041.5993082835621</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="6"/>
+        <v>45.448522204053916</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D16" s="2">
         <v>1</v>
       </c>
@@ -3242,39 +3898,79 @@
         <v>3017.4502254639801</v>
       </c>
       <c r="F16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4017.6994469597994</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4003.7228038115882</v>
       </c>
       <c r="H16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3990.1851648484521</v>
       </c>
       <c r="I16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4090.2595802492174</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4083.4730019709032</v>
       </c>
       <c r="K16" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4076.3115165788322</v>
       </c>
       <c r="L16" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4068.9130754407811</v>
       </c>
       <c r="M16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4061.3568776219404</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q16">
+        <f>G32</f>
+        <v>-4000.4312245851279</v>
+      </c>
+      <c r="R16" s="7">
+        <f t="shared" si="0"/>
+        <v>4000.4312245851279</v>
+      </c>
+      <c r="S16" s="5">
+        <f>$R$30</f>
+        <v>4080.3767415881071</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="U16" s="7">
+        <f>$R$25</f>
+        <v>3990.1851648484521</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="1"/>
+        <v>6.5858565648900367</v>
+      </c>
+      <c r="X16" s="7">
+        <f>$R$25</f>
+        <v>3990.1851648484521</v>
+      </c>
+      <c r="Y16" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="2"/>
+        <v>6.5858565648900367</v>
+      </c>
+      <c r="AA16" s="7">
+        <v>4048.1851648484521</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D17" s="2">
         <v>2</v>
       </c>
@@ -3282,52 +3978,256 @@
         <v>3020.7391131971299</v>
       </c>
       <c r="F17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4020.9883346929491</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4007.0116915447379</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3993.4740525816019</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4093.5484679823671</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4086.7618897040529</v>
       </c>
       <c r="K17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4079.6004043119819</v>
       </c>
       <c r="L17" s="11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4072.2019631739308</v>
       </c>
       <c r="M17" s="13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4064.6457653550901</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q17">
+        <f>G33</f>
+        <v>-4003.7228038115882</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="0"/>
+        <v>4003.7228038115882</v>
+      </c>
+      <c r="S17" s="14">
+        <f>$R$32</f>
+        <v>4086.9680010227571</v>
+      </c>
+      <c r="T17" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="U17" s="29">
+        <f>$R$14</f>
+        <v>3993.8399651504778</v>
+      </c>
+      <c r="V17" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="1"/>
+        <v>3.6548003020257056</v>
+      </c>
+      <c r="X17" s="29">
+        <f>$R$14</f>
+        <v>3993.8399651504778</v>
+      </c>
+      <c r="Y17" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="2"/>
+        <v>3.6548003020257056</v>
+      </c>
+      <c r="AA17" s="95">
+        <v>4051.8399651504778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q18">
+        <f>G34</f>
+        <v>-4007.0116915447379</v>
+      </c>
+      <c r="R18" s="95">
+        <f t="shared" si="0"/>
+        <v>4007.0116915447379</v>
+      </c>
+      <c r="S18" s="7">
+        <f>$R$35</f>
+        <v>3954.2770923921671</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="U18" s="27">
+        <f>$R$16</f>
+        <v>4000.4312245851279</v>
+      </c>
+      <c r="V18" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="1"/>
+        <v>6.5912594346500555</v>
+      </c>
+      <c r="X18" s="27">
+        <f>$R$16</f>
+        <v>4000.4312245851279</v>
+      </c>
+      <c r="Y18" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="2"/>
+        <v>6.5912594346500555</v>
+      </c>
+      <c r="AA18" s="7">
+        <v>4058.4312245851279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q19">
+        <f>H27</f>
+        <v>4047.5649295146177</v>
+      </c>
+      <c r="R19" s="14">
+        <f t="shared" si="0"/>
+        <v>4047.5649295146177</v>
+      </c>
+      <c r="S19" s="95">
+        <f>$R$37</f>
+        <v>3960.8629489570567</v>
+      </c>
+      <c r="T19" s="95" t="s">
+        <v>158</v>
+      </c>
+      <c r="U19" s="29">
+        <f>$R$18</f>
+        <v>4007.0116915447379</v>
+      </c>
+      <c r="V19" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="1"/>
+        <v>6.5804669596100211</v>
+      </c>
+      <c r="X19" s="29">
+        <f>$R$18</f>
+        <v>4007.0116915447379</v>
+      </c>
+      <c r="Y19" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="2"/>
+        <v>6.5804669596100211</v>
+      </c>
+      <c r="AA19" s="95">
+        <v>4065.0116915447379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="E20" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q20">
+        <f>H28</f>
+        <v>4050.8592068530488</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="0"/>
+        <v>4050.8592068530488</v>
+      </c>
+      <c r="S20" s="5">
+        <f>$R$39</f>
+        <v>4076.8871454060131</v>
+      </c>
+      <c r="T20" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="U20" s="27">
+        <f>$R$7</f>
+        <v>4011.1135903949094</v>
+      </c>
+      <c r="V20" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="1"/>
+        <v>4.1018988501714375</v>
+      </c>
+      <c r="X20" s="27">
+        <f>$R$7</f>
+        <v>4011.1135903949094</v>
+      </c>
+      <c r="Y20" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="2"/>
+        <v>4.1018988501714375</v>
+      </c>
+      <c r="AA20" s="7">
+        <v>4069.1135903949094</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="F21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q21">
+        <f>H29</f>
+        <v>4054.1507860795082</v>
+      </c>
+      <c r="R21" s="13">
+        <f t="shared" si="0"/>
+        <v>4054.1507860795082</v>
+      </c>
+      <c r="S21" s="14">
+        <f>$R$41</f>
+        <v>4083.4730019709032</v>
+      </c>
+      <c r="T21" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="U21" s="29">
+        <f>$R$9</f>
+        <v>4017.6994469597994</v>
+      </c>
+      <c r="V21" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="1"/>
+        <v>6.5858565648900367</v>
+      </c>
+      <c r="X21" s="29">
+        <f>$R$9</f>
+        <v>4017.6994469597994</v>
+      </c>
+      <c r="Y21" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="2"/>
+        <v>6.5858565648900367</v>
+      </c>
+      <c r="AA21" s="95">
+        <v>4075.6994469597994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -3337,8 +4237,48 @@
       <c r="K22" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q22">
+        <f>H30</f>
+        <v>-3980.3023261873418</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="0"/>
+        <v>3980.3023261873418</v>
+      </c>
+      <c r="S22" s="7">
+        <f>$R$44</f>
+        <v>3964.7328551226683</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="U22" s="14">
+        <f>$R$64</f>
+        <v>4058.0652983954801</v>
+      </c>
+      <c r="V22" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="1"/>
+        <v>40.365851435680725</v>
+      </c>
+      <c r="X22" s="14">
+        <f>$R$64</f>
+        <v>4058.0652983954801</v>
+      </c>
+      <c r="Y22" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="2"/>
+        <v>40.365851435680725</v>
+      </c>
+      <c r="AA22" s="14">
+        <v>4116.0652983954806</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>-1092</v>
       </c>
@@ -3348,16 +4288,104 @@
       <c r="K23" s="9">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q23">
+        <f>H31</f>
+        <v>-3983.5993082835621</v>
+      </c>
+      <c r="R23" s="95">
+        <f t="shared" si="0"/>
+        <v>3983.5993082835621</v>
+      </c>
+      <c r="S23" s="14">
+        <f>$R$46</f>
+        <v>4066.4286779177219</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="U23" s="14">
+        <f>$R$55</f>
+        <v>4062.327218875891</v>
+      </c>
+      <c r="V23" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="W23" s="122">
+        <f>U23-U22</f>
+        <v>4.2619204804109359</v>
+      </c>
+      <c r="X23" s="14">
+        <f>$R$55</f>
+        <v>4062.327218875891</v>
+      </c>
+      <c r="Y23" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" si="2"/>
+        <v>4.2619204804109359</v>
+      </c>
+      <c r="AA23" s="14">
+        <v>4120.327218875891</v>
+      </c>
+      <c r="AB23">
+        <f>ABS($AA$24-AA23)</f>
+        <v>2.3185464791986305</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="G24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q24">
+        <f>H32</f>
+        <v>-3986.8935856219919</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="0"/>
+        <v>3986.8935856219919</v>
+      </c>
+      <c r="S24" s="5">
+        <f>$R$48</f>
+        <v>4073.0199373523719</v>
+      </c>
+      <c r="T24" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="U24" s="5">
+        <f>$R$66</f>
+        <v>4064.6457653550901</v>
+      </c>
+      <c r="V24" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="W24" s="11">
+        <f>U24-U23</f>
+        <v>2.3185464791990853</v>
+      </c>
+      <c r="X24" s="5">
+        <f>$R$66</f>
+        <v>4064.6457653550901</v>
+      </c>
+      <c r="Y24" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" si="2"/>
+        <v>2.3185464791990853</v>
+      </c>
+      <c r="AA24" s="5">
+        <v>4122.6457653550897</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" ref="AB24:AB25" si="7">ABS($AA$24-AA24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="F25" s="2">
         <v>-1</v>
       </c>
@@ -3382,8 +4410,56 @@
       <c r="M25" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q25">
+        <f>H33</f>
+        <v>-3990.1851648484521</v>
+      </c>
+      <c r="R25" s="7">
+        <f t="shared" si="0"/>
+        <v>3990.1851648484521</v>
+      </c>
+      <c r="S25" s="14">
+        <f>$R$50</f>
+        <v>4079.6004043119819</v>
+      </c>
+      <c r="T25" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="U25" s="14">
+        <f>$R$46</f>
+        <v>4066.4286779177219</v>
+      </c>
+      <c r="V25" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="W25" s="123">
+        <f t="shared" si="1"/>
+        <v>1.7829125626317364</v>
+      </c>
+      <c r="X25" s="14">
+        <f>$R$46</f>
+        <v>4066.4286779177219</v>
+      </c>
+      <c r="Y25" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="2"/>
+        <v>1.7829125626317364</v>
+      </c>
+      <c r="AA25" s="14">
+        <v>4124.4286779177219</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" si="7"/>
+        <v>1.7829125626321911</v>
+      </c>
+      <c r="AC25">
+        <f>ABS($AA$26-AA25)</f>
+        <v>2.4843975230596698</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -3414,8 +4490,52 @@
       <c r="M26" s="10">
         <v>48.093347842039599</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q26">
+        <f>H34</f>
+        <v>-3993.4740525816019</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="0"/>
+        <v>3993.4740525816019</v>
+      </c>
+      <c r="S26" s="95">
+        <f>$R$51</f>
+        <v>3968.8370189222896</v>
+      </c>
+      <c r="T26" s="95" t="s">
+        <v>162</v>
+      </c>
+      <c r="U26" s="5">
+        <f>$R$57</f>
+        <v>4068.9130754407811</v>
+      </c>
+      <c r="V26" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="W26" s="18">
+        <f>U26-U25</f>
+        <v>2.484397523059215</v>
+      </c>
+      <c r="X26" s="5">
+        <f>$R$57</f>
+        <v>4068.9130754407811</v>
+      </c>
+      <c r="Y26" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" si="2"/>
+        <v>2.484397523059215</v>
+      </c>
+      <c r="AA26" s="5">
+        <v>4126.9130754407815</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" ref="AC26:AC27" si="8">ABS($AA$26-AA26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D27" s="2">
         <v>-1</v>
       </c>
@@ -3423,39 +4543,83 @@
         <v>-5020.2998688990901</v>
       </c>
       <c r="F27" s="13">
-        <f t="shared" ref="F27:M34" si="1">F$9-$E27 +$A$23</f>
+        <f t="shared" ref="F27:M34" si="9">F$9-$E27 +$A$23</f>
         <v>4020.0506474032709</v>
       </c>
       <c r="G27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4034.0272905514821</v>
       </c>
       <c r="H27" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4047.5649295146177</v>
       </c>
       <c r="I27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3947.4905141138534</v>
       </c>
       <c r="J27" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3954.2770923921671</v>
       </c>
       <c r="K27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3961.4385777842381</v>
       </c>
       <c r="L27" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3968.8370189222896</v>
       </c>
       <c r="M27" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3976.3932167411294</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q27">
+        <f>I27</f>
+        <v>3947.4905141138534</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="0"/>
+        <v>3947.4905141138534</v>
+      </c>
+      <c r="S27" s="7">
+        <f>$R$53</f>
+        <v>3975.4228754871792</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="U27" s="5">
+        <f>$R$48</f>
+        <v>4073.0199373523719</v>
+      </c>
+      <c r="V27" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="W27" s="119">
+        <f>U27-U26</f>
+        <v>4.1068619115908405</v>
+      </c>
+      <c r="X27" s="5">
+        <f>$R$48</f>
+        <v>4073.0199373523719</v>
+      </c>
+      <c r="Y27" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" si="2"/>
+        <v>4.1068619115908405</v>
+      </c>
+      <c r="AA27" s="5">
+        <v>4131.0199373523719</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="8"/>
+        <v>4.1068619115903857</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="9" t="s">
         <v>2</v>
       </c>
@@ -3472,39 +4636,83 @@
         <v>-5023.5941462375204</v>
       </c>
       <c r="F28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4023.3449247417011</v>
       </c>
       <c r="G28" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4037.3215678899123</v>
       </c>
       <c r="H28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4050.8592068530488</v>
       </c>
       <c r="I28" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3950.7847914522836</v>
       </c>
       <c r="J28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3957.5713697305973</v>
       </c>
       <c r="K28" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3964.7328551226683</v>
       </c>
       <c r="L28" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3972.1312962607199</v>
       </c>
       <c r="M28" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3979.6874940795597</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q28">
+        <f>I28</f>
+        <v>3950.7847914522836</v>
+      </c>
+      <c r="R28" s="95">
+        <f t="shared" si="0"/>
+        <v>3950.7847914522836</v>
+      </c>
+      <c r="S28" s="14">
+        <f>$R$55</f>
+        <v>4062.327218875891</v>
+      </c>
+      <c r="T28" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="U28" s="5">
+        <f>$R$39</f>
+        <v>4076.8871454060131</v>
+      </c>
+      <c r="V28" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="W28" s="119">
+        <f>U28-U27</f>
+        <v>3.8672080536412068</v>
+      </c>
+      <c r="X28" s="5">
+        <f>$R$39</f>
+        <v>4076.8871454060131</v>
+      </c>
+      <c r="Y28" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" si="2"/>
+        <v>3.8672080536412068</v>
+      </c>
+      <c r="AA28" s="5">
+        <v>4134.8871454060136</v>
+      </c>
+      <c r="AB28">
+        <f>ABS($AA$28-AA28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D29" s="2">
         <v>1</v>
       </c>
@@ -3512,39 +4720,87 @@
         <v>-5026.8857254639797</v>
       </c>
       <c r="F29" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4026.6365039681605</v>
       </c>
       <c r="G29" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4040.6131471163717</v>
       </c>
       <c r="H29" s="13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>4054.1507860795082</v>
       </c>
       <c r="I29" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3954.0763706787429</v>
       </c>
       <c r="J29" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3960.8629489570567</v>
       </c>
       <c r="K29" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3968.0244343491277</v>
       </c>
       <c r="L29" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3975.4228754871792</v>
       </c>
       <c r="M29" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>3982.979073306019</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q29">
+        <f>I29</f>
+        <v>3954.0763706787429</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="0"/>
+        <v>3954.0763706787429</v>
+      </c>
+      <c r="S29" s="5">
+        <f>$R$57</f>
+        <v>4068.9130754407811</v>
+      </c>
+      <c r="T29" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="U29" s="14">
+        <f>$R$50</f>
+        <v>4079.6004043119819</v>
+      </c>
+      <c r="V29" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="W29" s="18">
+        <f>U29-U28</f>
+        <v>2.7132589059688144</v>
+      </c>
+      <c r="X29" s="14">
+        <f>$R$50</f>
+        <v>4079.6004043119819</v>
+      </c>
+      <c r="Y29" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="2"/>
+        <v>2.7132589059688144</v>
+      </c>
+      <c r="AA29" s="14">
+        <v>4137.6004043119819</v>
+      </c>
+      <c r="AB29">
+        <f>ABS($AA$28-AA29)</f>
+        <v>2.7132589059683596</v>
+      </c>
+      <c r="AC29">
+        <f>ABS($AA$30-AA29)</f>
+        <v>0.77633727612465009</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D30" s="2">
         <v>-2</v>
       </c>
@@ -3552,39 +4808,86 @@
         <v>3007.5673868028698</v>
       </c>
       <c r="F30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4007.8166082986891</v>
       </c>
       <c r="G30" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-3993.8399651504778</v>
       </c>
       <c r="H30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-3980.3023261873418</v>
       </c>
       <c r="I30" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4080.3767415881071</v>
       </c>
       <c r="J30" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4073.5901633097928</v>
       </c>
       <c r="K30" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4066.4286779177219</v>
       </c>
       <c r="L30" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4059.0302367796708</v>
       </c>
       <c r="M30" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4051.4740389608301</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="N30" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q30">
+        <f>I30</f>
+        <v>-4080.3767415881071</v>
+      </c>
+      <c r="R30" s="5">
+        <f t="shared" si="0"/>
+        <v>4080.3767415881071</v>
+      </c>
+      <c r="S30" s="95">
+        <f>$R$60</f>
+        <v>3979.6874940795597</v>
+      </c>
+      <c r="T30" s="95" t="s">
+        <v>165</v>
+      </c>
+      <c r="U30" s="5">
+        <f>$R$30</f>
+        <v>4080.3767415881071</v>
+      </c>
+      <c r="V30" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="W30" s="124">
+        <f>U30-U29</f>
+        <v>0.77633727612510484</v>
+      </c>
+      <c r="X30" s="5">
+        <f>$R$30</f>
+        <v>4080.3767415881071</v>
+      </c>
+      <c r="Y30" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="2"/>
+        <v>0.77633727612510484</v>
+      </c>
+      <c r="AA30" s="5">
+        <v>4138.3767415881066</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" ref="AC30:AC31" si="10">ABS($AA$30-AA30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="D31" s="2">
         <v>-1</v>
       </c>
@@ -3592,39 +4895,86 @@
         <v>3010.8643688990901</v>
       </c>
       <c r="F31" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4011.1135903949094</v>
       </c>
       <c r="G31" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-3997.1369472466981</v>
       </c>
       <c r="H31" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-3983.5993082835621</v>
       </c>
       <c r="I31" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4083.6737236843273</v>
       </c>
       <c r="J31" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4076.8871454060131</v>
       </c>
       <c r="K31" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4069.7256600139422</v>
       </c>
       <c r="L31" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4062.327218875891</v>
       </c>
       <c r="M31" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4054.7710210570503</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="N31" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q31">
+        <f>I31</f>
+        <v>-4083.6737236843273</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="0"/>
+        <v>4083.6737236843273</v>
+      </c>
+      <c r="S31" s="14">
+        <f>$R$64</f>
+        <v>4058.0652983954801</v>
+      </c>
+      <c r="T31" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="U31" s="14">
+        <f>$R$41</f>
+        <v>4083.4730019709032</v>
+      </c>
+      <c r="V31" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="W31">
+        <f>U31-U30</f>
+        <v>3.0962603827961175</v>
+      </c>
+      <c r="X31" s="14">
+        <f>$R$41</f>
+        <v>4083.4730019709032</v>
+      </c>
+      <c r="Y31" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="2"/>
+        <v>3.0962603827961175</v>
+      </c>
+      <c r="AA31" s="14">
+        <v>4141.4730019709032</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="10"/>
+        <v>3.0962603827965722</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="9" t="s">
         <v>2</v>
       </c>
@@ -3641,39 +4991,79 @@
         <v>3014.1586462375199</v>
       </c>
       <c r="F32" s="17">
+        <f t="shared" si="9"/>
+        <v>-4014.4078677333391</v>
+      </c>
+      <c r="G32" s="15">
+        <f t="shared" si="9"/>
+        <v>-4000.4312245851279</v>
+      </c>
+      <c r="H32" s="17">
+        <f t="shared" si="9"/>
+        <v>-3986.8935856219919</v>
+      </c>
+      <c r="I32" s="18">
+        <f t="shared" si="9"/>
+        <v>-4086.9680010227571</v>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="9"/>
+        <v>-4080.1814227444429</v>
+      </c>
+      <c r="K32" s="19">
+        <f t="shared" si="9"/>
+        <v>-4073.0199373523719</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="9"/>
+        <v>-4065.6214962143208</v>
+      </c>
+      <c r="M32" s="18">
+        <f t="shared" si="9"/>
+        <v>-4058.0652983954801</v>
+      </c>
+      <c r="Q32">
+        <f>I32</f>
+        <v>-4086.9680010227571</v>
+      </c>
+      <c r="R32" s="14">
+        <f t="shared" si="0"/>
+        <v>4086.9680010227571</v>
+      </c>
+      <c r="S32" s="5">
+        <f>$R$66</f>
+        <v>4064.6457653550901</v>
+      </c>
+      <c r="T32" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="U32" s="14">
+        <f>$R$32</f>
+        <v>4086.9680010227571</v>
+      </c>
+      <c r="V32" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="W32" s="120">
         <f t="shared" si="1"/>
-        <v>-4014.4078677333391</v>
-      </c>
-      <c r="G32" s="15">
-        <f t="shared" si="1"/>
-        <v>-4000.4312245851279</v>
-      </c>
-      <c r="H32" s="17">
-        <f t="shared" si="1"/>
-        <v>-3986.8935856219919</v>
-      </c>
-      <c r="I32" s="18">
-        <f t="shared" si="1"/>
-        <v>-4086.9680010227571</v>
-      </c>
-      <c r="J32" s="6">
-        <f t="shared" si="1"/>
-        <v>-4080.1814227444429</v>
-      </c>
-      <c r="K32" s="19">
-        <f t="shared" si="1"/>
-        <v>-4073.0199373523719</v>
-      </c>
-      <c r="L32" s="6">
-        <f t="shared" si="1"/>
-        <v>-4065.6214962143208</v>
-      </c>
-      <c r="M32" s="18">
-        <f t="shared" si="1"/>
-        <v>-4058.0652983954801</v>
-      </c>
-    </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+        <v>3.494999051853938</v>
+      </c>
+      <c r="X32" s="14">
+        <f>$R$32</f>
+        <v>4086.9680010227571</v>
+      </c>
+      <c r="Y32" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="2"/>
+        <v>3.494999051853938</v>
+      </c>
+      <c r="AA32" s="14">
+        <v>4144.9680010227567</v>
+      </c>
+    </row>
+    <row r="33" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D33" s="2">
         <v>1</v>
       </c>
@@ -3681,39 +5071,50 @@
         <v>3017.4502254639801</v>
       </c>
       <c r="F33" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4017.6994469597994</v>
       </c>
       <c r="G33" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4003.7228038115882</v>
       </c>
       <c r="H33" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-3990.1851648484521</v>
       </c>
       <c r="I33" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4090.2595802492174</v>
       </c>
       <c r="J33" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4083.4730019709032</v>
       </c>
       <c r="K33" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4076.3115165788322</v>
       </c>
       <c r="L33" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4068.9130754407811</v>
       </c>
       <c r="M33" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4061.3568776219404</v>
       </c>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q33">
+        <f>I33</f>
+        <v>-4090.2595802492174</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="0"/>
+        <v>4090.2595802492174</v>
+      </c>
+      <c r="W33" s="25" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D34" s="2">
         <v>2</v>
       </c>
@@ -3721,39 +5122,53 @@
         <v>3020.7391131971299</v>
       </c>
       <c r="F34" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4020.9883346929491</v>
       </c>
       <c r="G34" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4007.0116915447379</v>
       </c>
       <c r="H34" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-3993.4740525816019</v>
       </c>
       <c r="I34" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4093.5484679823671</v>
       </c>
       <c r="J34" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4086.7618897040529</v>
       </c>
       <c r="K34" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4079.6004043119819</v>
       </c>
       <c r="L34" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4072.2019631739308</v>
       </c>
       <c r="M34" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>-4064.6457653550901</v>
       </c>
-    </row>
-    <row r="35" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q34">
+        <f>I34</f>
+        <v>-4093.5484679823671</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="0"/>
+        <v>4093.5484679823671</v>
+      </c>
+      <c r="V34" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+    </row>
+    <row r="35" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="17"/>
@@ -3761,19 +5176,55 @@
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
+      <c r="K35" s="17" t="s">
+        <v>169</v>
+      </c>
       <c r="L35" s="6"/>
       <c r="M35" s="17"/>
-    </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q35">
+        <f>J27</f>
+        <v>3954.2770923921671</v>
+      </c>
+      <c r="R35" s="7">
+        <f t="shared" si="0"/>
+        <v>3954.2770923921671</v>
+      </c>
+      <c r="T35" t="s">
+        <v>177</v>
+      </c>
+      <c r="V35" s="116" t="s">
+        <v>172</v>
+      </c>
+      <c r="W35" s="116"/>
+      <c r="X35" s="116"/>
+      <c r="Y35" s="116"/>
+    </row>
+    <row r="36" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E36" t="s">
         <v>83</v>
       </c>
       <c r="H36" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="K36" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q36">
+        <f>J28</f>
+        <v>3957.5713697305973</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="0"/>
+        <v>3957.5713697305973</v>
+      </c>
+      <c r="V36" s="121" t="s">
+        <v>173</v>
+      </c>
+      <c r="W36" s="121"/>
+      <c r="X36" s="121"/>
+      <c r="Y36" s="121"/>
+    </row>
+    <row r="37" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E37" s="25"/>
       <c r="F37" s="26" t="s">
         <v>56</v>
@@ -3793,14 +5244,25 @@
       <c r="M37" s="37">
         <v>-1040</v>
       </c>
-    </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q37">
+        <f>J29</f>
+        <v>3960.8629489570567</v>
+      </c>
+      <c r="R37" s="95">
+        <f t="shared" si="0"/>
+        <v>3960.8629489570567</v>
+      </c>
+      <c r="V37" s="95" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E38" s="25">
         <f>F27</f>
         <v>4020.0506474032709</v>
       </c>
       <c r="F38" s="25">
-        <f t="shared" ref="F38:F67" si="2">ABS(E38)</f>
+        <f t="shared" ref="F38:F67" si="11">ABS(E38)</f>
         <v>4020.0506474032709</v>
       </c>
       <c r="G38" s="25"/>
@@ -3816,14 +5278,28 @@
       <c r="M38" s="25">
         <v>3931.5993082835621</v>
       </c>
-    </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q38">
+        <f>J30</f>
+        <v>-4073.5901633097928</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="0"/>
+        <v>4073.5901633097928</v>
+      </c>
+      <c r="T38" t="s">
+        <v>178</v>
+      </c>
+      <c r="V38" s="119" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E39" s="25">
         <f>G28</f>
         <v>4037.3215678899123</v>
       </c>
       <c r="F39" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4037.3215678899123</v>
       </c>
       <c r="G39" s="25"/>
@@ -3839,14 +5315,25 @@
       <c r="M39" s="25">
         <v>3938.1851648484521</v>
       </c>
-    </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q39">
+        <f>J31</f>
+        <v>-4076.8871454060131</v>
+      </c>
+      <c r="R39" s="5">
+        <f t="shared" si="0"/>
+        <v>4076.8871454060131</v>
+      </c>
+      <c r="V39" s="120" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E40" s="25">
         <f>H29</f>
         <v>4054.1507860795082</v>
       </c>
       <c r="F40" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4054.1507860795082</v>
       </c>
       <c r="G40" s="25"/>
@@ -3862,14 +5349,22 @@
       <c r="M40" s="25">
         <v>3941.8399651504778</v>
       </c>
-    </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q40">
+        <f>J32</f>
+        <v>-4080.1814227444429</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="0"/>
+        <v>4080.1814227444429</v>
+      </c>
+    </row>
+    <row r="41" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E41" s="25">
         <f>I30</f>
         <v>-4080.3767415881071</v>
       </c>
       <c r="F41" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4080.3767415881071</v>
       </c>
       <c r="G41" s="25"/>
@@ -3885,14 +5380,22 @@
       <c r="M41" s="25">
         <v>3948.4312245851279</v>
       </c>
-    </row>
-    <row r="42" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q41">
+        <f>J33</f>
+        <v>-4083.4730019709032</v>
+      </c>
+      <c r="R41" s="14">
+        <f t="shared" si="0"/>
+        <v>4083.4730019709032</v>
+      </c>
+    </row>
+    <row r="42" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E42" s="25">
         <f>J31</f>
         <v>-4076.8871454060131</v>
       </c>
       <c r="F42" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4076.8871454060131</v>
       </c>
       <c r="G42" s="25"/>
@@ -3908,14 +5411,22 @@
       <c r="M42" s="25">
         <v>3955.0116915447379</v>
       </c>
-    </row>
-    <row r="43" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q42">
+        <f>J34</f>
+        <v>-4086.7618897040529</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="0"/>
+        <v>4086.7618897040529</v>
+      </c>
+    </row>
+    <row r="43" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E43" s="25">
         <f>K32</f>
         <v>-4073.0199373523719</v>
       </c>
       <c r="F43" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4073.0199373523719</v>
       </c>
       <c r="G43" s="25"/>
@@ -3931,14 +5442,22 @@
       <c r="M43" s="25">
         <v>3959.1135903949094</v>
       </c>
-    </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q43">
+        <f>K27</f>
+        <v>3961.4385777842381</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="0"/>
+        <v>3961.4385777842381</v>
+      </c>
+    </row>
+    <row r="44" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E44" s="25">
         <f>L33</f>
         <v>-4068.9130754407811</v>
       </c>
       <c r="F44" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4068.9130754407811</v>
       </c>
       <c r="G44" s="25"/>
@@ -3954,14 +5473,22 @@
       <c r="M44" s="25">
         <v>3965.6994469597994</v>
       </c>
-    </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q44">
+        <f>K28</f>
+        <v>3964.7328551226683</v>
+      </c>
+      <c r="R44" s="7">
+        <f t="shared" si="0"/>
+        <v>3964.7328551226683</v>
+      </c>
+    </row>
+    <row r="45" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E45" s="25">
         <f>M34</f>
         <v>-4064.6457653550901</v>
       </c>
       <c r="F45" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4064.6457653550901</v>
       </c>
       <c r="G45" s="25"/>
@@ -3977,14 +5504,22 @@
       <c r="M45" s="25">
         <v>4002.7847914522836</v>
       </c>
-    </row>
-    <row r="46" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q45">
+        <f>K29</f>
+        <v>3968.0244343491277</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="0"/>
+        <v>3968.0244343491277</v>
+      </c>
+    </row>
+    <row r="46" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E46" s="25">
         <f>I28</f>
         <v>3950.7847914522836</v>
       </c>
       <c r="F46" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3950.7847914522836</v>
       </c>
       <c r="G46" s="25"/>
@@ -4000,14 +5535,22 @@
       <c r="M46" s="25">
         <v>4006.0652983954801</v>
       </c>
-    </row>
-    <row r="47" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q46">
+        <f>K30</f>
+        <v>-4066.4286779177219</v>
+      </c>
+      <c r="R46" s="14">
+        <f t="shared" si="0"/>
+        <v>4066.4286779177219</v>
+      </c>
+    </row>
+    <row r="47" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E47" s="25">
         <f>J27</f>
         <v>3954.2770923921671</v>
       </c>
       <c r="F47" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3954.2770923921671</v>
       </c>
       <c r="G47" s="25"/>
@@ -4023,14 +5566,22 @@
       <c r="M47" s="25">
         <v>4006.2770923921671</v>
       </c>
-    </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q47">
+        <f>K31</f>
+        <v>-4069.7256600139422</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="0"/>
+        <v>4069.7256600139422</v>
+      </c>
+    </row>
+    <row r="48" spans="4:25" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" s="25">
         <f>J29</f>
         <v>3960.8629489570567</v>
       </c>
       <c r="F48" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3960.8629489570567</v>
       </c>
       <c r="G48" s="25" t="s">
@@ -4050,14 +5601,22 @@
       <c r="M48" s="28">
         <v>4010.327218875891</v>
       </c>
-    </row>
-    <row r="49" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q48">
+        <f>K32</f>
+        <v>-4073.0199373523719</v>
+      </c>
+      <c r="R48" s="5">
+        <f t="shared" si="0"/>
+        <v>4073.0199373523719</v>
+      </c>
+    </row>
+    <row r="49" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E49" s="25">
         <f>K28</f>
         <v>3964.7328551226683</v>
       </c>
       <c r="F49" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3964.7328551226683</v>
       </c>
       <c r="G49" s="25" t="s">
@@ -4077,14 +5636,22 @@
       <c r="M49" s="30">
         <v>4012.6457653550901</v>
       </c>
-    </row>
-    <row r="50" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q49">
+        <f>K33</f>
+        <v>-4076.3115165788322</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="0"/>
+        <v>4076.3115165788322</v>
+      </c>
+    </row>
+    <row r="50" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E50" s="25">
         <f>L27</f>
         <v>3968.8370189222896</v>
       </c>
       <c r="F50" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3968.8370189222896</v>
       </c>
       <c r="G50" s="25" t="s">
@@ -4104,14 +5671,22 @@
       <c r="M50" s="31">
         <v>4012.8629489570567</v>
       </c>
-    </row>
-    <row r="51" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q50">
+        <f>K34</f>
+        <v>-4079.6004043119819</v>
+      </c>
+      <c r="R50" s="14">
+        <f t="shared" si="0"/>
+        <v>4079.6004043119819</v>
+      </c>
+    </row>
+    <row r="51" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E51" s="25">
         <f>L29</f>
         <v>3975.4228754871792</v>
       </c>
       <c r="F51" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3975.4228754871792</v>
       </c>
       <c r="G51" s="25" t="s">
@@ -4134,14 +5709,22 @@
       <c r="M51" s="25">
         <v>4014.4286779177219</v>
       </c>
-    </row>
-    <row r="52" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q51">
+        <f>L27</f>
+        <v>3968.8370189222896</v>
+      </c>
+      <c r="R51" s="95">
+        <f t="shared" si="0"/>
+        <v>3968.8370189222896</v>
+      </c>
+    </row>
+    <row r="52" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E52" s="25">
         <f>M28</f>
         <v>3979.6874940795597</v>
       </c>
       <c r="F52" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3979.6874940795597</v>
       </c>
       <c r="G52" s="25" t="s">
@@ -4163,14 +5746,22 @@
       <c r="M52" s="27">
         <v>4016.7328551226683</v>
       </c>
-    </row>
-    <row r="53" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q52">
+        <f t="shared" ref="Q52:Q58" si="12">L28</f>
+        <v>3972.1312962607199</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="0"/>
+        <v>3972.1312962607199</v>
+      </c>
+    </row>
+    <row r="53" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E53" s="25">
         <f>F31</f>
         <v>-4011.1135903949094</v>
       </c>
       <c r="F53" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4011.1135903949094</v>
       </c>
       <c r="G53" s="25"/>
@@ -4183,14 +5774,22 @@
       <c r="K53" s="25"/>
       <c r="L53" s="25"/>
       <c r="M53" s="25"/>
-    </row>
-    <row r="54" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q53">
+        <f t="shared" si="12"/>
+        <v>3975.4228754871792</v>
+      </c>
+      <c r="R53" s="7">
+        <f t="shared" si="0"/>
+        <v>3975.4228754871792</v>
+      </c>
+    </row>
+    <row r="54" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E54" s="25">
         <f>G30</f>
         <v>-3993.8399651504778</v>
       </c>
       <c r="F54" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3993.8399651504778</v>
       </c>
       <c r="G54" s="25" t="s">
@@ -4212,14 +5811,22 @@
       <c r="M54" s="30">
         <v>4016.9130754407811</v>
       </c>
-    </row>
-    <row r="55" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q54">
+        <f t="shared" si="12"/>
+        <v>-4059.0302367796708</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="0"/>
+        <v>4059.0302367796708</v>
+      </c>
+    </row>
+    <row r="55" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E55" s="25">
         <f>G32</f>
         <v>-4000.4312245851279</v>
       </c>
       <c r="F55" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4000.4312245851279</v>
       </c>
       <c r="G55" s="25"/>
@@ -4232,14 +5839,22 @@
       <c r="K55" s="25"/>
       <c r="L55" s="25"/>
       <c r="M55" s="25"/>
-    </row>
-    <row r="56" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q55">
+        <f t="shared" si="12"/>
+        <v>-4062.327218875891</v>
+      </c>
+      <c r="R55" s="14">
+        <f t="shared" si="0"/>
+        <v>4062.327218875891</v>
+      </c>
+    </row>
+    <row r="56" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E56" s="25">
         <f>H31</f>
         <v>-3983.5993082835621</v>
       </c>
       <c r="F56" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3983.5993082835621</v>
       </c>
       <c r="G56" s="25" t="s">
@@ -4261,14 +5876,22 @@
       <c r="M56" s="29">
         <v>4020.8370189222896</v>
       </c>
-    </row>
-    <row r="57" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q56">
+        <f t="shared" si="12"/>
+        <v>-4065.6214962143208</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="0"/>
+        <v>4065.6214962143208</v>
+      </c>
+    </row>
+    <row r="57" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E57" s="25">
         <f>F33</f>
         <v>-4017.6994469597994</v>
       </c>
       <c r="F57" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4017.6994469597994</v>
       </c>
       <c r="G57" s="25" t="s">
@@ -4293,14 +5916,22 @@
       <c r="M57" s="30">
         <v>4021.0199373523719</v>
       </c>
-    </row>
-    <row r="58" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q57">
+        <f t="shared" si="12"/>
+        <v>-4068.9130754407811</v>
+      </c>
+      <c r="R57" s="5">
+        <f t="shared" si="0"/>
+        <v>4068.9130754407811</v>
+      </c>
+    </row>
+    <row r="58" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E58" s="25">
         <f>G34</f>
         <v>-4007.0116915447379</v>
       </c>
       <c r="F58" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4007.0116915447379</v>
       </c>
       <c r="G58" s="25" t="s">
@@ -4325,14 +5956,22 @@
       <c r="M58" s="30">
         <v>4024.8871454060131</v>
       </c>
-    </row>
-    <row r="59" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q58">
+        <f t="shared" si="12"/>
+        <v>-4072.2019631739308</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="0"/>
+        <v>4072.2019631739308</v>
+      </c>
+    </row>
+    <row r="59" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E59" s="25">
         <f>H33</f>
         <v>-3990.1851648484521</v>
       </c>
       <c r="F59" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>3990.1851648484521</v>
       </c>
       <c r="G59" s="33" t="s">
@@ -4354,14 +5993,22 @@
       <c r="M59" s="27">
         <v>4027.4228754871792</v>
       </c>
-    </row>
-    <row r="60" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q59">
+        <f>M27</f>
+        <v>3976.3932167411294</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="0"/>
+        <v>3976.3932167411294</v>
+      </c>
+    </row>
+    <row r="60" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E60" s="25">
         <f>K30</f>
         <v>-4066.4286779177219</v>
       </c>
       <c r="F60" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4066.4286779177219</v>
       </c>
       <c r="G60" s="25" t="s">
@@ -4386,14 +6033,22 @@
       <c r="M60" s="28">
         <v>4027.6004043119819</v>
       </c>
-    </row>
-    <row r="61" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q60">
+        <f t="shared" ref="Q60:Q65" si="13">M28</f>
+        <v>3979.6874940795597</v>
+      </c>
+      <c r="R60" s="95">
+        <f t="shared" si="0"/>
+        <v>3979.6874940795597</v>
+      </c>
+    </row>
+    <row r="61" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E61" s="25">
         <f>L31</f>
         <v>-4062.327218875891</v>
       </c>
       <c r="F61" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4062.327218875891</v>
       </c>
       <c r="G61" s="33" t="s">
@@ -4418,14 +6073,22 @@
       <c r="M61" s="30">
         <v>4028.3767415881071</v>
       </c>
-    </row>
-    <row r="62" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q61">
+        <f t="shared" si="13"/>
+        <v>3982.979073306019</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="0"/>
+        <v>3982.979073306019</v>
+      </c>
+    </row>
+    <row r="62" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E62" s="25">
         <f>M32</f>
         <v>-4058.0652983954801</v>
       </c>
       <c r="F62" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4058.0652983954801</v>
       </c>
       <c r="G62" s="33" t="s">
@@ -4447,14 +6110,22 @@
       <c r="M62" s="28">
         <v>4031.4730019709032</v>
       </c>
-    </row>
-    <row r="63" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q62">
+        <f t="shared" si="13"/>
+        <v>-4051.4740389608301</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="0"/>
+        <v>4051.4740389608301</v>
+      </c>
+    </row>
+    <row r="63" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E63" s="25">
         <f>I32</f>
         <v>-4086.9680010227571</v>
       </c>
       <c r="F63" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4086.9680010227571</v>
       </c>
       <c r="G63" s="25" t="s">
@@ -4477,14 +6148,22 @@
       <c r="M63" s="25">
         <v>4031.6874940795597</v>
       </c>
-    </row>
-    <row r="64" spans="5:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q63">
+        <f t="shared" si="13"/>
+        <v>-4054.7710210570503</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="0"/>
+        <v>4054.7710210570503</v>
+      </c>
+    </row>
+    <row r="64" spans="5:18" x14ac:dyDescent="0.55000000000000004">
       <c r="E64" s="25">
         <f>J33</f>
         <v>-4083.4730019709032</v>
       </c>
       <c r="F64" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4083.4730019709032</v>
       </c>
       <c r="G64" s="34" t="s">
@@ -4507,14 +6186,22 @@
         <v>4034.9680010227571</v>
       </c>
       <c r="O64" s="20"/>
-    </row>
-    <row r="65" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q64">
+        <f t="shared" si="13"/>
+        <v>-4058.0652983954801</v>
+      </c>
+      <c r="R64" s="14">
+        <f t="shared" si="0"/>
+        <v>4058.0652983954801</v>
+      </c>
+    </row>
+    <row r="65" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E65" s="25">
         <f>K34</f>
         <v>-4079.6004043119819</v>
       </c>
       <c r="F65" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4079.6004043119819</v>
       </c>
       <c r="G65" s="25" t="s">
@@ -4539,14 +6226,22 @@
       <c r="M65" s="32">
         <v>4072.0506474032709</v>
       </c>
-    </row>
-    <row r="66" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q65">
+        <f t="shared" si="13"/>
+        <v>-4061.3568776219404</v>
+      </c>
+      <c r="R65">
+        <f t="shared" si="0"/>
+        <v>4061.3568776219404</v>
+      </c>
+    </row>
+    <row r="66" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E66" s="25">
         <f>F29</f>
         <v>4026.6365039681605</v>
       </c>
       <c r="F66" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4026.6365039681605</v>
       </c>
       <c r="G66" s="25" t="s">
@@ -4571,14 +6266,22 @@
       <c r="M66" s="32">
         <v>4089.3215678899123</v>
       </c>
-    </row>
-    <row r="67" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q66">
+        <f>M34</f>
+        <v>-4064.6457653550901</v>
+      </c>
+      <c r="R66" s="5">
+        <f t="shared" si="0"/>
+        <v>4064.6457653550901</v>
+      </c>
+    </row>
+    <row r="67" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E67" s="25">
         <f>H27</f>
         <v>4047.5649295146177</v>
       </c>
       <c r="F67" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>4047.5649295146177</v>
       </c>
       <c r="G67" s="25" t="s">
@@ -4599,18 +6302,18 @@
         <v>4106.1507860795082</v>
       </c>
     </row>
-    <row r="68" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="H68" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="N69">
         <f>1/SQRT(3)</f>
         <v>0.57735026918962584</v>
       </c>
     </row>
-    <row r="70" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="J70">
         <f>SQRT(2*F75+1)</f>
         <v>1.7320508075688772</v>
@@ -4620,7 +6323,7 @@
         <v>0.44721359549995793</v>
       </c>
     </row>
-    <row r="71" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="G71" t="s">
         <v>31</v>
       </c>
@@ -4631,7 +6334,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="K72" s="48"/>
       <c r="L72" s="50">
         <v>0.5</v>
@@ -4643,7 +6346,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="73" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E73" s="26" t="s">
         <v>2</v>
       </c>
@@ -4680,12 +6383,14 @@
       <c r="S73" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="X73" s="22"/>
-      <c r="Y73" s="52" t="s">
+      <c r="T73" s="92"/>
+      <c r="U73" s="88"/>
+      <c r="Z73" s="22"/>
+      <c r="AA73" s="52" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E74" s="25">
         <v>2</v>
       </c>
@@ -4712,7 +6417,7 @@
         <v>5.7735026918962581E-2</v>
       </c>
       <c r="M74" s="25">
-        <f t="shared" ref="M74:M93" si="3">SQRT(2*F74+1)*L74*K74</f>
+        <f t="shared" ref="M74:M93" si="14">SQRT(2*F74+1)*L74*K74</f>
         <v>0</v>
       </c>
       <c r="N74" s="38"/>
@@ -4725,30 +6430,32 @@
         <v>4000.4312245851279</v>
       </c>
       <c r="S74" s="25">
-        <f t="shared" ref="S74:S90" si="4">R75-R74</f>
+        <f t="shared" ref="S74:S90" si="15">R75-R74</f>
         <v>6.5804669596100211</v>
       </c>
-      <c r="U74">
-        <v>1</v>
-      </c>
-      <c r="V74">
-        <v>1</v>
-      </c>
+      <c r="T74" s="25"/>
+      <c r="U74" s="25"/>
       <c r="W74">
         <v>1</v>
       </c>
-      <c r="X74" s="32">
+      <c r="X74">
+        <v>1</v>
+      </c>
+      <c r="Y74">
+        <v>1</v>
+      </c>
+      <c r="Z74" s="32">
         <v>4020.0506474032709</v>
       </c>
-      <c r="Y74" s="25">
-        <f t="shared" ref="Y74:Y80" si="5">X75-X74</f>
+      <c r="AA74" s="25">
+        <f t="shared" ref="AA74:AA80" si="16">Z75-Z74</f>
         <v>17.270920486641444</v>
       </c>
-      <c r="Z74" t="s">
+      <c r="AB74" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E75" s="25">
         <v>2</v>
       </c>
@@ -4775,7 +6482,7 @@
         <v>5.7735026918962581E-2</v>
       </c>
       <c r="M75" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>7.45E-3</v>
       </c>
       <c r="N75" s="38"/>
@@ -4789,24 +6496,26 @@
         <v>4007.0116915447379</v>
       </c>
       <c r="S75" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>4.1018988501714375</v>
       </c>
-      <c r="W75">
+      <c r="T75" s="25"/>
+      <c r="U75" s="25"/>
+      <c r="Y75">
         <v>2</v>
       </c>
-      <c r="X75" s="32">
+      <c r="Z75" s="32">
         <v>4037.3215678899123</v>
       </c>
-      <c r="Y75" s="25">
-        <f t="shared" si="5"/>
+      <c r="AA75" s="25">
+        <f t="shared" si="16"/>
         <v>16.829218189595849</v>
       </c>
-      <c r="Z75" s="93" t="s">
+      <c r="AB75" s="93" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E76" s="25">
         <v>2</v>
       </c>
@@ -4833,7 +6542,7 @@
         <v>5.7735026918962581E-2</v>
       </c>
       <c r="M76" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.5810000000000001E-2</v>
       </c>
       <c r="N76" s="40"/>
@@ -4847,30 +6556,32 @@
         <v>4011.1135903949094</v>
       </c>
       <c r="S76" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>6.5858565648900367</v>
       </c>
-      <c r="U76">
+      <c r="T76" s="117"/>
+      <c r="U76" s="118"/>
+      <c r="W76">
         <v>2</v>
       </c>
-      <c r="V76">
+      <c r="X76">
         <v>2</v>
       </c>
-      <c r="W76">
+      <c r="Y76">
         <v>3</v>
       </c>
-      <c r="X76" s="32">
+      <c r="Z76" s="32">
         <v>4054.1507860795082</v>
       </c>
-      <c r="Y76" s="25">
-        <f t="shared" si="5"/>
+      <c r="AA76" s="25">
+        <f t="shared" si="16"/>
         <v>10.494979275581954</v>
       </c>
-      <c r="Z76" t="s">
+      <c r="AB76" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E77" s="25">
         <v>2</v>
       </c>
@@ -4897,7 +6608,7 @@
         <v>5.7735026918962581E-2</v>
       </c>
       <c r="M77" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>5.2700000000000004E-3</v>
       </c>
       <c r="N77" s="40"/>
@@ -4911,27 +6622,29 @@
         <v>4017.6994469597994</v>
       </c>
       <c r="S77" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2.3512004434714981</v>
       </c>
-      <c r="V77">
+      <c r="T77" s="25"/>
+      <c r="U77" s="25"/>
+      <c r="X77">
         <v>3</v>
       </c>
-      <c r="W77">
+      <c r="Y77">
         <v>4</v>
       </c>
-      <c r="X77" s="30">
+      <c r="Z77" s="30">
         <v>4064.6457653550901</v>
       </c>
-      <c r="Y77" s="25">
-        <f t="shared" si="5"/>
+      <c r="AA77" s="25">
+        <f t="shared" si="16"/>
         <v>4.2673100856909514</v>
       </c>
-      <c r="Z77" t="s">
+      <c r="AB77" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E78" s="25">
         <v>1</v>
       </c>
@@ -4958,7 +6671,7 @@
         <v>0.22360679774997896</v>
       </c>
       <c r="M78" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>3.5360337950873712E-2</v>
       </c>
       <c r="N78" s="42"/>
@@ -4972,24 +6685,26 @@
         <v>4020.0506474032709</v>
       </c>
       <c r="S78" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>17.270920486641444</v>
       </c>
-      <c r="W78">
+      <c r="T78" s="25"/>
+      <c r="U78" s="25"/>
+      <c r="Y78">
         <v>5</v>
       </c>
-      <c r="X78" s="30">
+      <c r="Z78" s="30">
         <v>4068.9130754407811</v>
       </c>
-      <c r="Y78" s="25">
-        <f t="shared" si="5"/>
+      <c r="AA78" s="25">
+        <f t="shared" si="16"/>
         <v>4.1068619115908405</v>
       </c>
-      <c r="Z78" t="s">
+      <c r="AB78" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="79" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="D79" t="s">
         <v>102</v>
       </c>
@@ -5020,7 +6735,7 @@
         <v>0.22360679774997896</v>
       </c>
       <c r="M79" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>3.5360337950873712E-2</v>
       </c>
       <c r="N79" s="40"/>
@@ -5033,30 +6748,32 @@
         <v>4037.3215678899123</v>
       </c>
       <c r="S79" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>16.829218189595849</v>
       </c>
-      <c r="U79">
+      <c r="T79" s="25"/>
+      <c r="U79" s="25"/>
+      <c r="W79">
         <v>3</v>
       </c>
-      <c r="V79">
+      <c r="X79">
         <v>4</v>
       </c>
-      <c r="W79">
+      <c r="Y79">
         <v>6</v>
       </c>
-      <c r="X79" s="30">
+      <c r="Z79" s="30">
         <v>4073.0199373523719</v>
       </c>
-      <c r="Y79" s="25">
-        <f t="shared" si="5"/>
+      <c r="AA79" s="25">
+        <f t="shared" si="16"/>
         <v>3.8672080536412068</v>
       </c>
-      <c r="Z79" t="s">
+      <c r="AB79" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E80" s="25">
         <v>1</v>
       </c>
@@ -5083,7 +6800,7 @@
         <v>0.22360679774997896</v>
       </c>
       <c r="M80" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>7.0720675901747423E-2</v>
       </c>
       <c r="N80" s="38"/>
@@ -5097,24 +6814,26 @@
         <v>4054.1507860795082</v>
       </c>
       <c r="S80" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>3.9145123159719333</v>
       </c>
-      <c r="W80">
+      <c r="T80" s="25"/>
+      <c r="U80" s="25"/>
+      <c r="Y80">
         <v>7</v>
       </c>
-      <c r="X80" s="30">
+      <c r="Z80" s="30">
         <v>4076.8871454060131</v>
       </c>
-      <c r="Y80" s="25">
-        <f t="shared" si="5"/>
+      <c r="AA80" s="25">
+        <f t="shared" si="16"/>
         <v>3.4895961820939192</v>
       </c>
-      <c r="Z80" t="s">
+      <c r="AB80" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="D81" t="s">
         <v>102</v>
       </c>
@@ -5145,7 +6864,7 @@
         <v>0.22360679774997896</v>
       </c>
       <c r="M81" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>3.5360337950873712E-2</v>
       </c>
       <c r="N81" s="40"/>
@@ -5158,21 +6877,23 @@
         <v>4058.0652983954801</v>
       </c>
       <c r="S81" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>4.2619204804109359</v>
       </c>
-      <c r="V81">
+      <c r="T81" s="25"/>
+      <c r="U81" s="25"/>
+      <c r="X81">
         <v>5</v>
       </c>
-      <c r="X81" s="30">
+      <c r="Z81" s="30">
         <v>4080.3767415881071</v>
       </c>
-      <c r="Y81" s="25"/>
-      <c r="Z81" t="s">
+      <c r="AA81" s="25"/>
+      <c r="AB81" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E82" s="25">
         <v>1</v>
       </c>
@@ -5199,7 +6920,7 @@
         <v>0.22360679774997896</v>
       </c>
       <c r="M82" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>3.5360337950873712E-2</v>
       </c>
       <c r="N82" s="42"/>
@@ -5213,11 +6934,13 @@
         <v>4062.327218875891</v>
       </c>
       <c r="S82" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2.3185464791990853</v>
       </c>
-    </row>
-    <row r="83" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T82" s="25"/>
+      <c r="U82" s="25"/>
+    </row>
+    <row r="83" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E83" s="25">
         <v>2</v>
       </c>
@@ -5243,25 +6966,27 @@
         <v>0.1</v>
       </c>
       <c r="M83" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.0910893696210225E-2</v>
       </c>
       <c r="N83" s="40"/>
       <c r="O83" s="40"/>
       <c r="P83" s="41"/>
       <c r="Q83" s="25">
-        <f t="shared" ref="Q83:Q93" si="6">Q82+1</f>
+        <f t="shared" ref="Q83:Q93" si="17">Q82+1</f>
         <v>8</v>
       </c>
       <c r="R83" s="30">
         <v>4064.6457653550901</v>
       </c>
       <c r="S83" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>1.7829125626317364</v>
       </c>
-    </row>
-    <row r="84" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T83" s="25"/>
+      <c r="U83" s="25"/>
+    </row>
+    <row r="84" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E84" s="25">
         <v>2</v>
       </c>
@@ -5287,25 +7012,27 @@
         <v>0.1</v>
       </c>
       <c r="M84" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.3362742233538744E-2</v>
       </c>
       <c r="N84" s="38"/>
       <c r="O84" s="38"/>
       <c r="P84" s="41"/>
       <c r="Q84" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="R84" s="28">
         <v>4066.4286779177219</v>
       </c>
       <c r="S84" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2.484397523059215</v>
       </c>
-    </row>
-    <row r="85" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T84" s="25"/>
+      <c r="U84" s="25"/>
+    </row>
+    <row r="85" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E85" s="25">
         <v>2</v>
       </c>
@@ -5331,25 +7058,27 @@
         <v>0.1</v>
       </c>
       <c r="M85" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>2.6725484467077489E-2</v>
       </c>
       <c r="N85" s="38"/>
       <c r="O85" s="42"/>
       <c r="P85" s="43"/>
       <c r="Q85" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
       <c r="R85" s="30">
         <v>4068.9130754407811</v>
       </c>
       <c r="S85" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>4.1068619115908405</v>
       </c>
-    </row>
-    <row r="86" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T85" s="25"/>
+      <c r="U85" s="25"/>
+    </row>
+    <row r="86" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E86" s="25">
         <v>2</v>
       </c>
@@ -5375,25 +7104,27 @@
         <v>0.1</v>
       </c>
       <c r="M86" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.0910893696210225E-2</v>
       </c>
       <c r="N86" s="40"/>
       <c r="O86" s="40"/>
       <c r="P86" s="41"/>
       <c r="Q86" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
       <c r="R86" s="30">
         <v>4073.0199373523719</v>
       </c>
       <c r="S86" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>3.8672080536412068</v>
       </c>
-    </row>
-    <row r="87" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T86" s="25"/>
+      <c r="U86" s="25"/>
+    </row>
+    <row r="87" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E87" s="25">
         <v>2</v>
       </c>
@@ -5419,21 +7150,21 @@
         <v>0.1</v>
       </c>
       <c r="M87" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.3362742233538744E-2</v>
       </c>
       <c r="N87" s="38"/>
       <c r="O87" s="38"/>
       <c r="P87" s="43"/>
       <c r="Q87" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
       <c r="R87" s="30">
         <v>4076.8871454060131</v>
       </c>
       <c r="S87" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>2.7132589059688144</v>
       </c>
       <c r="T87">
@@ -5441,7 +7172,7 @@
         <v>3.4895961820939192</v>
       </c>
     </row>
-    <row r="88" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E88" s="25">
         <v>2</v>
       </c>
@@ -5467,25 +7198,27 @@
         <v>0.1</v>
       </c>
       <c r="M88" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>2.6725484467077489E-2</v>
       </c>
       <c r="N88" s="42"/>
       <c r="O88" s="42"/>
       <c r="P88" s="43"/>
       <c r="Q88" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>13</v>
       </c>
       <c r="R88" s="35">
         <v>4079.6004043119819</v>
       </c>
       <c r="S88" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>0.77633727612510484</v>
       </c>
-    </row>
-    <row r="89" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T88" s="25"/>
+      <c r="U88" s="25"/>
+    </row>
+    <row r="89" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E89" s="25">
         <v>2</v>
       </c>
@@ -5511,25 +7244,27 @@
         <v>0.1</v>
       </c>
       <c r="M89" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.3362742233538744E-2</v>
       </c>
       <c r="N89" s="38"/>
       <c r="O89" s="38"/>
       <c r="P89" s="43"/>
       <c r="Q89" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>14</v>
       </c>
       <c r="R89" s="30">
         <v>4080.3767415881071</v>
       </c>
       <c r="S89" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>3.0962603827961175</v>
       </c>
-    </row>
-    <row r="90" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T89" s="25"/>
+      <c r="U89" s="25"/>
+    </row>
+    <row r="90" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E90" s="25">
         <v>2</v>
       </c>
@@ -5555,25 +7290,27 @@
         <v>0.1</v>
       </c>
       <c r="M90" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.0910893696210225E-2</v>
       </c>
       <c r="N90" s="40"/>
       <c r="O90" s="40"/>
       <c r="P90" s="41"/>
       <c r="Q90" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>15</v>
       </c>
       <c r="R90" s="28">
         <v>4083.4730019709032</v>
       </c>
       <c r="S90" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>3.494999051853938</v>
       </c>
-    </row>
-    <row r="91" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T90" s="25"/>
+      <c r="U90" s="25"/>
+    </row>
+    <row r="91" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E91" s="25">
         <v>2</v>
       </c>
@@ -5599,22 +7336,24 @@
         <v>0.1</v>
       </c>
       <c r="M91" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>2.6725484467077489E-2</v>
       </c>
       <c r="N91" s="38"/>
       <c r="O91" s="42"/>
       <c r="P91" s="39"/>
       <c r="Q91" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>16</v>
       </c>
       <c r="R91" s="28">
         <v>4086.9680010227571</v>
       </c>
       <c r="S91" s="25"/>
-    </row>
-    <row r="92" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="T91" s="25"/>
+      <c r="U91" s="25"/>
+    </row>
+    <row r="92" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E92" s="25">
         <v>2</v>
       </c>
@@ -5640,18 +7379,18 @@
         <v>0.1</v>
       </c>
       <c r="M92" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.3362742233538744E-2</v>
       </c>
       <c r="N92" s="38"/>
       <c r="O92" s="38"/>
       <c r="P92" s="41"/>
       <c r="Q92" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="E93" s="25">
         <v>2</v>
       </c>
@@ -5677,25 +7416,25 @@
         <v>0.1</v>
       </c>
       <c r="M93" s="25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>1.0910893696210225E-2</v>
       </c>
       <c r="N93" s="45"/>
       <c r="O93" s="45"/>
       <c r="P93" s="46"/>
       <c r="Q93" s="25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="17"/>
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="P94" s="23"/>
       <c r="Q94" s="23"/>
     </row>
-    <row r="95" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="K95" s="25"/>
     </row>
-    <row r="96" spans="4:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="4:28" x14ac:dyDescent="0.55000000000000004">
       <c r="L96" s="25"/>
     </row>
     <row r="97" spans="9:18" x14ac:dyDescent="0.55000000000000004">
@@ -5719,8 +7458,8 @@
       <c r="L102" s="25"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L106:L145">
-    <sortCondition ref="L106"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="X3:Y32">
+    <sortCondition ref="X2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5731,8 +7470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA73D89-17E0-437A-B9B8-7353842BB85C}">
   <dimension ref="A1:U101"/>
   <sheetViews>
-    <sheetView topLeftCell="C36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7553,7 +9292,7 @@
         <v>4054.0652983954801</v>
       </c>
       <c r="H72" s="102">
-        <f t="shared" ref="H72:H75" si="18">$G$73-G72</f>
+        <f>$G$73-G72</f>
         <v>8.5487684028066724E-2</v>
       </c>
       <c r="J72" t="s">
@@ -7592,7 +9331,7 @@
         <v>4054.1507860795082</v>
       </c>
       <c r="H73" s="98">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="H72:H75" si="18">$G$73-G73</f>
         <v>0</v>
       </c>
       <c r="I73" t="s">

</xml_diff>